<commit_message>
Get daily reddit data: Tue Sep  3 08:10:13 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_09_08.xlsx
+++ b/data/2024_09_08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C483"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3100 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1f7tuc3</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>The winter coming</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wq3nlffpjmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1f7qwoy</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>How do you get your polish to last more then 2 days?</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f7qwoy/how_do_you_get_your_polish_to_last_more_then_2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1f7sst6</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>What should I use to buff my nails for gel polish?</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f7sst6/what_should_i_use_to_buff_my_nails_for_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1f7ssct</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally tried non sticky hard gel for moulding 3D things! </t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7ssct</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1f7rq2j</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Got my last set of the summer 🦋</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06pgmj640jmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1f7qouo</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Genuine question as first time acrylic haver.</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7qouo</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1f7pu94</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Trying to get into the spooky mood</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7pu94</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1f7pqsi</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Can salon fix a tear in my nail?</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5utolh1jgimd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1f7pmi3</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>For those who use press ons what glue remover do you use?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f7pmi3/for_those_who_use_press_ons_what_glue_remover_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1f7p11p</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>I loved them, do you like them?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qlf7mtd6aimd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1f7p0bo</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Back to school nails</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4lc45l00aimd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1f7ouqn</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>i did my own nails !</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxrxze5m8imd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1f7oh1j</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>First time diy acrylic</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mxr75wz95imd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1f7o4kg</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Update* salvaged what I could. really appreciate all the advice and support!</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7btvqcb2imd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1f7nq06</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Hand models &amp; manicures</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7nq06</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1f7lynd</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>What color nails should I get for my parent’s wedding? This is the color of my dress. The nail color needs to be more nude/demure. Nothing flashy. Any ideas?</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45urdbycjhmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1f7mp08</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>which nail is your fav? mine is def the cheetah print 🐆</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/326p9brqphmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1f7mhmw</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first set in a minute, my new tech popped off </t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qwpgw0znhmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1f7me6g</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I finished painting this Beetlejuice aquarium nail 😭 finally </t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/32am9q94nhmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1f7lt5o</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Press on glue help?</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f7lt5o/press_on_glue_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1f7ks85</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Just admiring these and made a new friend</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ck8vnd7j9hmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1f7kqzd</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kitty nails </t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fw5emex89hmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1f7kisp</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Halloween I feel you</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7kisp</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1f7ke69</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just did my first set of acrylic's! </t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7ke69</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1f7k9dq</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>nails with wave design.</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kc8xpnff5hmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1f7k675</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>I gave my nail tech a sketch</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7k675</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1f7jz57</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Why does my builder gel lift from the nail tip?</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f7jz57/why_does_my_builder_gel_lift_from_the_nail_tip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1f7jz6l</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Just wanted to share the Beetlejuice nails I did! So excited for the movie!</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mb0lilo53hmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1f7jsbq</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Rough nails</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f7jsbq/rough_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1f7jjxr</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Stiletto lovers - what kind of dish gloves are you wearing?</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f7jjxr/stiletto_lovers_what_kind_of_dish_gloves_are_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1f7jhg3</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Sally Hansen MEGA Strengh HARDENER, not the color line</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f7jhg3/sally_hansen_mega_strengh_hardener_not_the_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1f7j9yi</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Holo Taco crushed holo water marble love the look of the holo crystals! Base polish Suger Rush-water marble polishes Jam Session-Sunshine Crush-Sour Note-Blue Rizzler-Electric Sweetener-Pop Rocker</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7j9yi</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1f7j81b</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>My nail tech and I are excited for fall</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gb5c8wadxgmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1f7fzyz</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My newest set.  </t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f7fzyz/my_newest_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1f7eok0</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Nail glue technique?</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5c2x3yk70gmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1f7g4ph</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Broke a natural nail. Time to chop ‘em off. </t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7g4ph</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1f7gozy</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on love </t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7gozy</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1f7ixfc</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help me order wedding nails </t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7ixfc</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1f7iwrq</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Can’t stop looking at these chrome bad boys</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9gkv6nyugmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1f7hyaj</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>not sure how i feel about this new set. what do you guys think? 🥲</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7hyaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1f7htc4</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Something for fall </t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7htc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1f7hsc8</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Pretty in lilac 💅</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jsp11lpmgmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1f7hruk</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Some of he sets I’ve gotten done this year ❣️</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7hruk</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1f7hmit</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Yellow, another option</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rx7kw7whlgmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1f7hkbl</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Kokoist lamp not curing properly</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f7hkbl/kokoist_lamp_not_curing_properly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1f7hgi5</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying to go from round/square to almond (slowly), but it feels really difficult </t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zxvd4bp8kgmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1f7hf08</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>First autumn set 🍂🍁</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7hf08</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1f7h070</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Glamnetics falling off - glue issue?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f7h070/glamnetics_falling_off_glue_issue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1f7gtbj</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Ready to fly, through the blue sky</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxziu0lkfgmd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1f7gm12</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>First attempt at dip nails</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7gm12</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1f7gg7f</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>First time with black and loving it!</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ockp6zpwcgmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1f7f21j</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Look what I found under my bed!!!</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4l8qzahu2gmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1f7fmmh</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>First set, since taking a break over the summer</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7fmmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1f7fm8s</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>It's me again with a new design for you. What do you think about? 🧚🏻🤍</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7fm8s</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1f7fahz</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Neapolitan ice cream nails!!!</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7fahz</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1f7f2eq</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>At home DIY extras to Salon Gel Nails?</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ee7l3zex2gmd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1f7exdk</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Looking for Illimite polishes from Live Love Polish</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f7exdk/looking_for_illimite_polishes_from_live_love/</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1f7el7r</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>How do we feel about the see through/jelly nails?</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7el7r</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1f7ehvw</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Natural Nails: Advice on Strengthening!</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f7ehvw/natural_nails_advice_on_strengthening/</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1f7e9zw</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Beetlejuice! Beetlejuice! Beetlejuice!</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7e9zw</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1f7e42a</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Ready for Fall! 🍂🍁</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/31zd4le4wfmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1f7d83n</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pre Halloween nails </t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybu69hiupfmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1f7cuhw</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Nails not drying?</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f7cuhw/nails_not_drying/</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1f769vl</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help me decide what’s best for my nails! </t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xnduq0aiaemd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1f72tmn</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! Nails lifting/peeling constantly </t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f72tmn</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1f748zf</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Best gel option for thin bendy nails?</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f748zf/best_gel_option_for_thin_bendy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1f78vni</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Other "daylight" UV non-gel polishes?</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f78vni/other_daylight_uv_nongel_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1f79of2</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Newbie to extensions - help needed</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f79of2/newbie_to_extensions_help_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1f7c3pd</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>My baby cousins nails</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/37svk5gxhfmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1f7c1q2</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🩵 💙  🩵 💙 </t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7c1q2</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1f7c1hs</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>GR is way better than iPhone</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7c1hs</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1f7bqew</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>A set i did myself 💅🏻</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7bqew</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1f7bnm7</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Wedding nails</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u95epepuefmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1f7b7f6</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you search for your beauty master when moving in the new country/city? </t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l3n9vl3mbfmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1f7aysn</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Today I say goodbye to this gorgeous set :(</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7aysn</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1f7auoo</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>green chrome russian mani! 💚</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7auoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1f7ant3</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Gel toes, nails too long</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f7ant3/gel_toes_nails_too_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1f7a42n</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>How did you find your nail tech?</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f7a42n/how_did_you_find_your_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1f7a1s1</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Help using nail drying spray</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f7a1s1/help_using_nail_drying_spray/</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1f79pti</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>You all rocking with these or no?</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f79pti</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1f78u3e</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ready for Autumn 🍂 </t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f78u3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1f78o0b</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello September </t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lw9buf83temd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1f77yo0</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>When your nail tech always gets you together 🤗</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f77yo0</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1f77uff</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glam boys represent! 💅🏽 </t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f77uff</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1f77omv</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Shrinkage - wtf?</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvaric9olemd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1f77ja6</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Guess the movie/serie</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f77ja6</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1f77hvz</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gotta love an all natural Barbie set </t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4p0lhtl7kemd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1f774g3</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Last summer set of the year!</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/64n9s2dchemd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1f76r9o</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Nails stickers! How would you call this green color? I mixed 1/6 of "C-Hill Out" in a whole bottle of "Hard Drive Me Crazy" (Sally Hansen)</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bafgt16geemd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1f76lgf</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Mother daughter nail pictures</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f76lgf</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1f76k7h</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my mix and match nails </t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/knhf6mnucemd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1f765v0</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>My new manicure nail cutting game</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1jm7guj9emd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1f75z1w</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Sick all day yesterday but at least my nails looked good 🎀</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0zkqmgax7emd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1f75pf5</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>KBShimmer - Get Off My Tail</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f75pf5</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1f75fuy</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stitch and Angel handpainted </t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvwd4gjy2emd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1f758rf</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>How to fix nail split</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/skt1w5pz0emd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1f74fkj</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think? </t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f74fkj</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1f72nw5</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>wedding nails</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f72nw5</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1f728d2</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>how to make nail polish stay on longer?</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f728d2/how_to_make_nail_polish_stay_on_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1f71v0y</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t xml:space="preserve">like them? </t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p17pbheuycmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1f7ucsx</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Purple skittle-ish</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhprssu5wjmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1f7snal</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opi x Wicked </t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7snal</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1f7rc1p</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What am I doing wrong? </t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hsovzujzvimd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1f7r3z1</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Does anybody know a dupe for the Chanel 181?</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3xeixs6ntimd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1f7qr9m</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Love this international nail color</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7qr9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1f7qquk</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Lurid’s “To the Force and Pressure of Time” is so gorgeous 😍</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sqe5htq0qimd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1f7q8q2</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Corpse Bride Mani + Spooky Haul</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7q8q2</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1f7q0eq</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blooming Azalea </t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7q0eq</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1f7pg67</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Holo Taco Crimson Void w/ Matte Top Coat 🧛🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7pg67</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1f7pa3r</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Rogue lacquer - matcha latte</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7pvp4udcimd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1f7p03y</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Snail Nails</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7p03y</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1f7oxy1</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail polish and depression </t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f7oxy1/nail_polish_and_depression/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1f7ov40</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>PPU- Swamp Gloss Swift and Saddled</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7ov40</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1f7ohwo</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel extensions keep popping off:( Need advice </t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f7ohwo/gel_extensions_keep_popping_off_need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1f7o6s3</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>I posted the horrible blue chrome mani a few weeks ago. I’m getting a little better. Took everything you guys said and tried to go from there!</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8pzycxu2imd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1f7m0jf</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>I rarely do skittles but this one has me thinking I should do them more often 💚🩷</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7m0jf</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1f7lr5v</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Orly Ruby for my first fall mani</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7lr5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1f7lbh5</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What polish do you choose for your birthday?? </t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7lbh5</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1f7l1e9</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>So satisfying to have finally filled out my first all-PPU swatch wheel!</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0ilvftenbhmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1f7kyf1</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>🌑new moon nails🌑</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2lct0dnyahmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1f7knvd</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Slow launch of fall colors</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7knvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1f7kbtl</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Wowwwwwweee last hurrah before fall nails ❤️</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7kbtl</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1f7k8p7</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Drunkfairy polish question </t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f7k8p7/drunkfairy_polish_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1f7k6iy</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Liquid Fire 🔥 for when you’re craving fall but still love summer </t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7k6iy</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1f7juwr</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Thoughts on a mauve/lavender/gold shimmer or holo polish? Inspired by the Disney "Earidescent" color.</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mw6w4d1h1hmd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1f7jago</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Holo Taco crushed holo water marble love the look of the holo crystals! Base polish Suger Rush-water marble polishes Jam Session-Sunshine Crush-Sour Note-Blue Rizzler-Electric Sweetener-Pop Rocker</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7jago</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1f7j8kt</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>kbshimmer frequent flyer vs out of sequins</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f7j8kt/kbshimmer_frequent_flyer_vs_out_of_sequins/</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1f7ih6s</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phoenix - Eclipse </t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7ih6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1f7ieqo</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blooming Azalea for the end of summer </t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2ymh6nd3rgmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1f7id2d</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Taking inspo from my fave TJs coffee</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7id2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1f7i06y</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Labor day sales? </t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f7i06y/labor_day_sales/</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1f7h2k6</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Always prettier than I remembered </t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7h2k6</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1f7erdg</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Orly Terra Nova (PR) 🤠🐎 </t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wbfx9cfs0gmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1f7dmkn</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Beetlejuice! Beetlejuice! Beetlejuice!</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o92lshxqsfmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1f7dkin</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Help! Experiencing burnout as a beginner</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f7dkin/help_experiencing_burnout_as_a_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1f7d2t0</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Remains one of my faves ♥️💙💜</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cizvgjqvofmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1f7ctfa</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Damn you BKL</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5f17jpx2nfmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1f7cspx</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Everything Taco &amp; Dove Jelly Sandwich </t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpkyrkywmfmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1f7c5ub</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Where to buy Whatcha Laquer polishes?</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f7c5ub/where_to_buy_whatcha_laquer_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1f7bn7p</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Jelly + Flakie Sunset Gradient 🌅</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7bn7p</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1f7blwb</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>I'm shifting into fall mode 🖤</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7blwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1f7bfzm</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>My husband surprised me with some ILNPs ❤️😭</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7bfzm</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1f7b8rl</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>From Summer to Fall 🌻🍁</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7b8rl</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1f7aia4</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dr. Pepper red with a smattering of mascara flakes on top ❤️ </t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cfkwf59k6fmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1f7a7sa</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Top of the Taupes!</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/rKaaLnG</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1f7a6pu</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>we have sandviper at home</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/opd85q694fmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1f7a6dd</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>ILNP jellies 😍😍</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7a6dd</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1f7a5f0</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>BKL - Your Heart is My Heart</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7a5f0</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1f79fzt</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Tried a flakie bomb polish for the first time - loving it!</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f79fzt</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1f79fvr</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Venus flytrap 😍</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f79fvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1f794bo</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>ILNP Lily Velvetized</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f794bo</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1f78zeq</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Bright pink for the final days of summer</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f78zeq</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1f78kf6</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Looking for a dupe for MC's Dream Within a Dream</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f78kf6/looking_for_a_dupe_for_mcs_dream_within_a_dream/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1f78fzj</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Sky nails~</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f78fzj</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1f77ych</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Little chrome snake</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xn1b6o1qnemd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1f7738q</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Cirque Haze &amp; ILNP Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7738q</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1f76rri</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Patience and Shipping Question</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f76rri/patience_and_shipping_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1f76ntk</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wedding nail help? </t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3nak53bv9emd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1f761ie</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Flight of the Monarchs appreciation post #1737281</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f761ie</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1f75xx0</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>KBShimmer - Get Off My Tail</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f75xx0</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1f709ba</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>How to do nail extensions without gel</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f709ba/how_to_do_nail_extensions_without_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1f75fxg</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>ISO: Slate grey with silver shimmer (I want to match my cat)</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f75fxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1f737nz</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t xml:space="preserve">For the first time in 35 years I have nails I can be proud of. </t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f737nz</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1f731nl</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f731nl/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1f72bnt</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jewel Rainbow </t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f72bnt/jewel_rainbow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1f71whr</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>A possibly stupid question about "all-in-one" nail polishes</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f71whr/a_possibly_stupid_question_about_allinone_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1f7s005</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Hollow Knight Nails</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7s005</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1f7pa6w</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>🐻🍳</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pdk53aoecimd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1f7nd1o</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Beetlejuice set I did on myself! So excited for the movie!</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bv9rpwhkvhmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1f7mdrx</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I finished painting this Beetlejuice aquarium nail 😭 finally </t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w3k1ket0nhmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1f7j7m6</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>All my clients love this design in thousands of colors</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7j7m6</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1f7iz2d</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Haven't posted in a while</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikno00mgvgmd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1f7g8pb</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>My favorite nail design so far! Victorian-inspired!</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvm7u0mgbgmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1f7g2zc</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Always fulfilling the whims of my clients</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/il1inwtcagmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1f7ey3w</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Hand sculpted octopus with his treasures 🥺 one of my last summer sets ❤️</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7ey3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1f7bs46</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>HELP I received my nail art utensils and have no clue how some of them work</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mghmmk5rffmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1f7boyk</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Wedding nails!</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hs57rg54ffmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1f7a50p</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Beetlejuice! Beetlejuice! Beetlejuice!</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qfrcho9w3fmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1f79col</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Lots of Firsts!</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f79col</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1f786s6</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time with nail art </t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2k2i2ajpemd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1f77zau</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>which supplies a beginner should buy?</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1f77zau/which_supplies_a_beginner_should_buy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1f766my</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Round 2 of Pokémon nails! </t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f766my</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Sep  4 08:08:42 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_09_08.xlsx
+++ b/data/2024_09_08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C483"/>
+  <dimension ref="A1:C659"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8644,6 +8644,2998 @@
         </is>
       </c>
     </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1f8nosc</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Pink has always been my favorite color</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4mnrdzn41rmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1f8nlzx</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Red and Black! Always a good combo 😍❤️🖤</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jcyqvmd30rmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1f8n6ho</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Went for something a bit different, what do y’all think?</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2u5fsl3duqmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1f8mpai</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Getting better!</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2i7uq146oqmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1f8mit1</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Love my new nail Tech</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8mit1</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1f8l4mh</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>I used the teabag method</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xay0125l5qmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1f8dtja</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Bubbles in the polish… is this normal?</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8dtja</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1f8h3kp</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Help! 😩</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f8h3kp/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1f8kdhk</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Manifesting spooky season (+ bonus cursed pose pic I sent my husband)</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8kdhk</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1f8j84d</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>I wanted to show this wonder🩵💦🫧🌬️</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8j84d</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1f8iia4</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Throwback to this set I got for my Hawaii trip 🐚</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8iia4</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1f8ifhs</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set </t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4lkshv2mfpmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1f8ifh2</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Red of love</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f986rvslfpmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1f8hgn4</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Berry picking nails! 🫐🍓✨</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8hgn4</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1f8ha04</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>My nail tech wanted to do a Smiling Friends set and my god did she deliver</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8ha04</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1f8h9y0</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>ImPRESS nails:: I had never done a bold color before this set which I completed while waiting in line for a Mejuri store opening so I could try on jewelry</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bdzipuem5pmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1f8gw61</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Natural Nails</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3bkeds3a2pmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1f8gh2n</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>**URGENT** How to heal nails after gel</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f8gh2n/urgent_how_to_heal_nails_after_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1f8gke4</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any constructive feedback? </t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ziwgejbhzomd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1f8g07t</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did a much needed fill &amp; went a little crazy with the designs 🥲 </t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8g07t</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1f8fuuq</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>It's giving Lizzie McGuire vibes, even though that wasn't my intention...</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xos5uxotomd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1f8fudl</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried builder gel at home :) I'm obsessed </t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqjw6pcltomd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1f8fj42</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>💜</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/249lhc13romd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1f8f8ix</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New to nails and was purchasing a sizing kit wondering how to determine what my size is? </t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f8f8ix/new_to_nails_and_was_purchasing_a_sizing_kit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1f8ezw5</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Advice + best online tutorials for gel nails</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f8ezw5/advice_best_online_tutorials_for_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1f8exvl</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Let my gf do my nails </t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3jtms1wcmomd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1f8elkn</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>To cut or not cut my nails 😭</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pd0rzvimjomd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1f8empm</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Oh look, a strawberry 🍓</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2od60zujomd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1f8ekn2</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>blinding bbs! ⭐️</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2g0el2sejomd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1f8eht2</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Do you like them?</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bu9t1sasiomd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1f8eh80</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Disappearing Toenail Bed </t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bs88q6dniomd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1f8edl6</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>good glue for press ons??</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f8edl6/good_glue_for_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1f8ec8g</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Last week's and this weeks</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8ec8g</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1f8ebx2</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Nail suggestions for graduation?</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f8ebx2/nail_suggestions_for_graduation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1f8e9od</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Second set! </t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8e9od</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1f8dwl8</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>These green nails came out beautiful ✨</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/95secjxjdomd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1f8dz87</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>I love them but SOMETHING about these nails is not sitting right with me what is it? Helppppp ❤️</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8dz87</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1f8e7pc</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Newest set I did ✨</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6fxcps9gomd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1f8cf0w</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Best at-home option to seal tops of nails w/o damage</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f8cf0w/best_athome_option_to_seal_tops_of_nails_wo_damage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1f8cebx</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Acrylic Removal Rookie….is this right??</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f8cebx/acrylic_removal_rookieis_this_right/</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1f8c57h</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Old School Operation Game Nails</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tvr2hzmoynmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1f8cor9</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Hello! I want to share with you my nails this month, very 2000's style.</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2av2ofaq2omd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1f8bwcc</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Troubleshooting prematurely grown-out nails</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8bwcc</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1f8bm92</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does this nail shape look good on me? </t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8bm92</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1f8bf00</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>What do you think of my new set?</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/67ytg92ctnmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1f8bc0w</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Dipping powder maintenance?</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fo717xsssnmd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1f8ar5i</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Nail Tip Broken Under Gel Polish</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6k4m1n4nonmd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1f8b68a</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tortoise nails 🐢 </t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8b68a</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1f8b24e</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anniversary nails </t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/toqgltuuqnmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1f8ald0</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Update: I’m furious over my nails</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8ald0</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1f8akfk</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Au natureeeel - good? Tips on maintenance? </t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6rkplt9nnmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1f8ah3f</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>My tech’s 1st time using cat eye polish - love the result!</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ig0x8q0jmnmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1f88wfq</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Cracked nail advice pls</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f88wfq/cracked_nail_advice_pls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1f88ucw</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Is it me or is it the activator that I bought?</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f88ucw/is_it_me_or_is_it_the_activator_that_i_bought/</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1f86ygu</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>how do I know when to remove...</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cnf8zpfrxmmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1f8a2qb</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What nail shape is best for my hand? </t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wjit061qjnmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1f89er7</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Pre vs. Post-Chop!</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fly9qhtxenmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1f88xrf</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>First time with a new tech, and she killed it 😍</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ou2hg7hkbnmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1f88vrk</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Transitioning into Autumn with these gorgeous moody nails from OPI in "Como Se Llama?"</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xjyqtjz5bnmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1f87p0x</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Romantic </t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f87p0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1f87mpp</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Pink nails</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n5vns4di2nmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1f87emc</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Abstract Nail Art</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f87emc</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1f877m8</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Junk nails.</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gntbodijzmmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1f873t8</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My square nails won't stop breaking on the edges </t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f873t8/my_square_nails_wont_stop_breaking_on_the_edges/</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1f869ds</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tips on how to open necklace  clasps </t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qp3cze0wsmmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1f85xbu</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Latest Set 🩷 </t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ei0c0uiqmmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1f852eg</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Will I be able to shorten the length without having to remove them?</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3jj9577lkmmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1f84a3p</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Which shape suits me better? ❤️</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f84a3p</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1f83y3g</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>The color of my eyes, what do you think? ( I do not recommend smoking )</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0zcnxs5qcmmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1f803rx</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Cybersigilism nails, so proud of these🤭🪩</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f803rx</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1f81oer</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Peel-off base coat that doesn't turn gel polish "gummy"?</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f81oer/peeloff_base_coat_that_doesnt_turn_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1f82bet</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Avoiding acetone with gel nails</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f82bet/avoiding_acetone_with_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1f82j4m</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it normal to use normal nail glue for extensions? </t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f82j4m/is_it_normal_to_use_normal_nail_glue_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1f7tc4j</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Broke a natural nail. Time to chop ‘em off.</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7tc4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1f7wm91</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>HELP! My gel nails become discoloured within days?</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f7wm91/help_my_gel_nails_become_discoloured_within_days/</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1f8318m</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>How can I fix my broken nail?</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8318m</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1f82yi1</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Simple mani</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f82yi1</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1f82ufw</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time growing out almonds after years of rounded-square. Please give any advice. 🙏 I shaped these myself and they are still pretty short (for now). </t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f82ufw</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1f827h6</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>First spooky set of 2024</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t4h9kzo90mmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1f81t1c</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Still learning, but Love Them 💖</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yq5u70rbxlmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1f81da0</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Recommendation please- Nail glue that can be removed without acetone</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f81da0/recommendation_please_nail_glue_that_can_be/</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1f80roc</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Love this set</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lr4gjnjhplmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1f80l3b</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Help with Cleaning Up Gel</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f80l3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1f80cp1</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Russian Manicure. Glitter Base. French Tips. Chrome Finish. Short Square Shape. 💅</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f80cp1</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1f7zeue</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Very cutesy nails</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pu99bpewelmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1f7z3rw</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3D art practice 😅 </t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0ky5kucclmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1f7z104</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Gojo Satoru Nail Art ✨💙</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7z104</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1f7yyle</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween but make it spring(?) </t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvuowh95blmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1f7xn12</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Hey, trainee here! My first ever nail job, thoughts?</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7xn12</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1f7x523</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Shaping the C-curve ?</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7x523</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1f7wmok</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Post gel removal &amp; filing</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zknb3va8okmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1f7vyl9</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Electric Carnival Beetles Gel Polish 🖤</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7vyl9</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1f7v4zp</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>bro i miss this set so much 😭😭</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iicy9du26kmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1f8myuu</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How can I replace Sally Hansen brushes </t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f8myuu/how_can_i_replace_sally_hansen_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1f8mkqq</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Crackle toppers (update, I guess??)</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f8mkqq/crackle_toppers_update_i_guess/</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1f8kb9p</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Essie “Good as New” before &amp; after!</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8kb9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1f8k5o2</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Wedding Nails</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f8k5o2/wedding_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1f8k1p4</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My brain: If I don’t get this it’s the exact same thing as being opposed to bleeding disorder awareness, and choosing to do intentional harm to people w/ bleeding disorders </t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ilncvtrmupmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1f8jsv4</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Blue and white mani</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8jsv4</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1f8ijnj</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to finish gel nails when I don’t have a free edge? </t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ncr24x9mgpmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1f8ia9c</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I found an old pic of my nails! </t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8ia9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1f8i2y0</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Another Venus flytrap photo it’s just too stunning! </t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uraskg4kcpmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1f8hdh8</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Flowerchild &amp; treachery in the blue </t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ypkbzkpg6pmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1f8h1ji</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Finally long enough to paint!  Dashing Diva Gloss Violet Moonstone</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bb7hu9bl3pmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1f8gxx2</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirque Colors Delirium </t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nt06ruzo2pmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1f8gb9v</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Horseshoe Magnet 🧲 velvet nail effect, 30lb vs 13lb. Anyone try both and do you see a difference?</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y2u65snexomd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1f8fgvp</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Treachery </t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8fgvp</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1f8elyc</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Didn't intend to match my polish to my drink, but...</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2g9dewoiomd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1f8ehui</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>cat eye moment 🪩🩶🩷⭐️</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8ehui</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1f8e08l</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>If you could only wear one polish for the rest of your life, which one would it be?</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f8e08l/if_you_could_only_wear_one_polish_for_the_rest_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1f8dwmx</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Coke can inspired nails </t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8dwmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1f8d9fo</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Help with ID Orly nail polish</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/187bnfu17omd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1f8d2r2</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Layering for that depth </t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xu8ekso5omd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1f8d1oo</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>1926 Peggy Sage in Dark - No top coat required</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eigf9hag5omd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1f8cp4y</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Now you see me, now you don't! (Duochrome effect)</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8cp4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1f8cmos</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Green Jelly</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f8cmos/green_jelly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1f8cb67</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Discussion: Anyone ever feel like their nail length doesn’t match their body type or personality? </t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qt5vubdxznmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1f8bwgy</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Matte Appreciation Post</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8bwgy</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1f8bopp</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Super Difficult to capture this one</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8bopp</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1f8b0h7</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving Drown my demons </t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nmqo5mliqnmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1f8ajht</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Play Date w/ Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8ajht</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1f8a5la</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>In SoCal summer is far from over 🥵</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8a5la</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1f89xh1</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Shake Your Shamrock ☘️</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f89xh1</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1f89wzt</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Feeling a bit blue lately 💙</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dm6rg5kjinmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1f89nuw</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>My post-chop manicure that I did for my family camping trip :) Also my first time doing almonds!</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f89nuw</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1f89f8z</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Took a pic while waiting to pick up my Spouse from work</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ben1nhb1fnmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1f89dxb</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>How can I recreate these beauties at home?</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.tumblr.com/cultcieht/755389511952973824?source=share</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1f884dt</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Best brands for damaged weak nails</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f884dt/best_brands_for_damaged_weak_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1f87vdr</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Moody Nail Polish Recommendations</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f87vdr</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1f87u4s</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>I want to try a thermal! Suggestions?</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f87u4s/i_want_to_try_a_thermal_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1f87edn</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Phoenix Indie 'Bismuto' with the velvet technique</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wjtfbh6v0nmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1f87aks</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>5 days Glory-ious wear</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f87aks</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1f85jad</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Back to School✏️📓🍎📚🖍️</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f85jad</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1f851ly</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Finally got the horseshoe magnet...</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3ih6srbekmmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1f84x7s</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Nail Polish Bottles Chipping/Fading</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f84x7s</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1f84wpa</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>🏜⛰️SoutwestvVista⛰️🏜</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f84wpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1f84oi7</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Daughter of the Old Kingdom 👑 </t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f84oi7</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1f84o0t</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Thank You For Cleaning My Toilet (PPU June 2024)</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f84o0t</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1f84fcx</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>You ever just… stop and admire 🫧</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ms032ox3gmmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1f84a4t</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone know any good dupes for Opi “is that a spear in your pocket?” </t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dz4wuzv2fmmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1f840b7</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>What’s your favorite quick dry top coat?</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f840b7/whats_your_favorite_quick_dry_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1f83xu8</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>What are your favorite one coat colors?</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f83xu8/what_are_your_favorite_one_coat_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1f83eg1</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>SO PRETTY</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f83eg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1f83700</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Lumen Glass Stars Oops Batch Comparison</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f83700</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1f82v9q</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>I love Mooncat</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iq3rkcv25mmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1f82qaa</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>My going-back-to-work-postpartum mani</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bbwt8jy24mmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1f815d9</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>What did I do wrong? Why do my nails always look like this only two days after painting them?</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qiewpiadslmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1f810bp</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Holo Taco’s “Holo Cappucino”. Have been working so hard on my mani skills for the last year!</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uckj3cobrlmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1f80pyh</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Life as a Shrimp 🦐 at the beach </t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ihaoapg4plmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1f80pt8</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Top coat for glitter?</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f80pt8/top_coat_for_glitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1f800ic</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>✨ Periwinkle ✨</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f800ic</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1f7ygdo</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you search for your beauty master when moving in the new country/city? </t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f7ygdo/how_do_you_search_for_your_beauty_master_when/</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1f7z1ru</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Does this guava pink color and nail shape suit my hands?</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f7z1ru/does_this_guava_pink_color_and_nail_shape_suit_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1f7yol2</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Do I have problems?</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a6n8wt1q8lmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1f7wa80</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do UV lamps cause anyone else’s fingers to darken? </t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f7wa80/do_uv_lamps_cause_anyone_elses_fingers_to_darken/</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1f7vq0y</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Clear polish</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f7vq0y/clear_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1f7v4ui</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>I wanted to show off chamaeleon nails purple moon</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f7v4ui</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1f8ieqq</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Is there an improvement?</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8ieqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1f8ha1k</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Cat eye Chrome 3D Fold with Rainbow Flowers</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8ha1k</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1f8f9bh</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Natural nails and regular polish!!</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8f9bh</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1f8ewfz</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Let my gf do my nails</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gtb9u1g1momd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1f8e72n</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Newest set I did ✨</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d73rrjryfomd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1f8cpkl</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Hello! I want to share with you my nails this month, very 2000's style.</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dkzkc6dw2omd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1f8cfz0</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t xml:space="preserve">practicing nail art </t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8cfz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1f8b3dl</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tortoise nails 🐢 </t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8b3dl</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1f89vja</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>any tips with cleanly attaching gems and decals?</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f89vja</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1f88wvl</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>how to put pictures on nails like in this photo?</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22u2q21ebnmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1f85ygi</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Pretty in Pink 🩷</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ludbo6brqmmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1f85s86</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Demon Slayer Challenge</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4ad019kpmmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1f85rs1</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t xml:space="preserve">[iso] HELP ME FIND THIS PLATE </t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kwj1tvepmmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1f8559n</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>BEETLEJUICE INSPIRED CUSTOM PRESS ONS 🖤</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekg8uxh4lmmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1f8534d</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>First spooky set of 2024</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fjcjzjaqkmmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1f81edz</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The little animal crackers! Made them from hard gel! (Nails by me) </t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7emt0wkaulmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1f7yuyi</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spent five hours painting these lil mountains </t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0r3p9cu9almd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1f7yhz4</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you search for your beauty master when moving in the new country/city? </t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1f7yhz4/how_do_you_search_for_your_beauty_master_when/</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1f7wlin</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dipped in gold </t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cxf3yjctnkmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Sep  5 08:10:05 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_09_08.xlsx
+++ b/data/2024_09_08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C659"/>
+  <dimension ref="A1:C835"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11636,6 +11636,2998 @@
         </is>
       </c>
     </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1f9gren</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Bring back the coffin nail ⚰️ no</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wuvecg8o2ymd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1f9gkj1</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Help me with chrome! Left is black base, right is red base</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dy3pyju00ymd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1f9gjna</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>korilakkuma set ⋅˚♡‧ ೀ</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9gjna</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1f9fhgb</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Second try on press-on nails! I  like these.😍</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ednr4269mxmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1f9esq0</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t xml:space="preserve">more spoopy nails♥ </t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/918e22khexmd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1f9e4e9</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>would you guys recommend getting a kit for a beginner in acrylic nails or get items individually?</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ts2dma837xmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1f9d4fb</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>gel x set from last week 🤎</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fiu5kvjxwwmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1f9d21n</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>I’m digging them</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/051nf3kawwmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1f9b1xu</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Builder Gel</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2gsr56a1ewmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1f9al9g</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Salon! </t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9al9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1f9acjj</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>my diy press on nails i did the other day 🥹</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/opfa9c2s7wmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1f9a64a</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Using my babies to take nail photos 😂🧸</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9a64a</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1f9a1xo</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>What do you think of this design? I like it for Halloween and an angel costume or one that has white in it.</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/467iqm585wmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1f9a08i</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first time doing my own nails at home! </t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9a08i</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1f99zy1</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first time doing my own nails at home! </t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f99zy1</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1f99m72</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>By the seaside</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n8smpquj1wmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1f98nrr</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>What do nail techs use to clean feet?</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f98nrr/what_do_nail_techs_use_to_clean_feet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1f964xk</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Why does it look “wet” under my nails and how do I get rid of it?</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebfh3vk19vmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1f990gx</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Style butterfly🦋</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kvmgdfcdwvmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1f98ww8</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Spring ➡️ Fall Transition Nails</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f98ww8</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1f98l9r</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Decided to try a different shape, not sure how I feel about it yet lol</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f98l9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1f9826u</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>In memory of ❤️</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9826u</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1f98048</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Some of my summer sets😇</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f98048</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1f97npc</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue nails left or right ?? </t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f97npc</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1f96l2a</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Extra extra short glue press ons</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f96l2a/extra_extra_short_glue_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1f97296</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>First time trying press-ons! Open to feedback :)</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f97296</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1f96azs</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>3rd try with gel x!</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mxn9mraavmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1f967te</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First manicure since finishing chemo! </t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f967te</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1f96058</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First set! </t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f96058</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1f95udr</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>New nailss</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f95udr</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1f95raf</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>First attempt ever at builder gel!</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f95raf</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1f9567y</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Favorite tools/companies gel x tips/builder gel</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwwxe3wv1vmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1f94xz8</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>What iS The Difference Between The Two?</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f94xz8/what_is_the_difference_between_the_two/</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1f94usr</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>The Robin blue changes color</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f94usr</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1f94u3y</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What did I do wrong? </t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f94u3y</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1f94qqc</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t xml:space="preserve">They look so plain. I want to go back to the salon. But I can’t decide on anything. Some help please :( </t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fvh4ax9gyumd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1f94j4z</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>irresistible beauty of long nails</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f94j4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1f94iup</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>They remind me of Sailor Moon</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yx3hzlypwumd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1f93utx</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m kinda in shock right now </t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f93utx</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1f93lci</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Help with shape</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f93lci</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1f92pwy</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Press ons?</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f92pwy/press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1f930sw</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>please help me</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f930sw/please_help_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1f91uh8</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Color Help? Design by _OFF.THE.WALL.NAILS_ on Instagram </t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i688h1oedumd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1f91e65</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>My first nails inspired by the anime series Naruto. They are not perfect, but they are one of my favorites.</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j9fwbv69aumd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1f91lnd</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do we like the flowers? </t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f91lnd</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1f91eup</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Curving nails</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f91eup</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1f91ebh</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Long or Short Nails?</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wcbmc44aaumd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1f9143s</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It's blue AND green. </t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9143s</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1f910g4</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Can I use press ons with my unusual nail shape?</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u2t4c7vi7umd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1f90xoh</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need Nail Ideas! </t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tmvralqz6umd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1f90n8i</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>how to achieve better coffin shape?</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60wpyzsx4umd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1f90b73</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>First time doing clouds</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f90b73</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1f8zx7n</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>When should I remove my gel nails to minimise the damage?</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f8zx7n/when_should_i_remove_my_gel_nails_to_minimise_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1f8zv2x</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How can i deal with an overgrown hyponychium? </t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f8zv2x/how_can_i_deal_with_an_overgrown_hyponychium/</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1f8zqqv</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>1st manicure</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8zqqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1f8zn4d</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Favorite nail polishes you can buy in-store? </t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f8zn4d/favorite_nail_polishes_you_can_buy_instore/</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1f8z4pp</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>A beginner did my nails. How did she do ? (She had 3 months of experience, semi-permanent on natural nails)</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8z4pp</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1f8z6jl</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Beginner... any tips?</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f8z6jl/beginner_any_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1f8z51p</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>First time growing out my nails - advice for nail shape?</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8z51p</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1f8ywyi</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>OPI 'This Color's Making Waves'</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nyic3ljpstmd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1f8yk9x</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>How do I get my nails to grow thicker and not bend?</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wuq4lm9qtmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1f8yl7f</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Is this normal after a dry/russian manicure?</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6ij4d1gqtmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1f8ydov</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Natural nail tear - just a little panicked 😭</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kq368r40ptmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1f8x5u3</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which nail shape is stronger? </t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f8x5u3/which_nail_shape_is_stronger/</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1f8wfy2</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>💙 Fine China 🤍</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0gnepdo6btmd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1f8qy5o</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What I asked for vs what I got </t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8qy5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1f8tts4</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Swan lake nails inspired by monet </t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8tts4</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1f8ul4u</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Please help me find a toe color that works with these nails!</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/41s60u5lxsmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1f8vusy</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>🏁 🖤 My attempt vs inspo (IG @brushedbyb_ )</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8vusy</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1f8mxh4</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>what is this?😨</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4d6q9y62rqmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1f8rphk</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>How do I find a good salon?</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f8rphk/how_do_i_find_a_good_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1f8ss9s</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Glamnetic “Ma Damn”</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kex9jtlnjsmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1f8vx96</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did it! First time doing my own nails! </t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8vx96</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1f8v6h6</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Best opi white gel</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f8v6h6/best_opi_white_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1f8uwus</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>lil french</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8uwus</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1f8uwdf</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>I don't know about these</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8uwdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1f8uqtv</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>pink'n'shiny (been a long while since my last set 🥴)</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8uqtv</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1f8ub2t</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>🍋</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/95n0tfvjvsmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1f8u95a</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Help! Broke a nail and now I don't know what shape to do.</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r00626b4vsmd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1f8u5mm</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Suddenly craving chocolate..</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8u5mm</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1f8tz3m</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>diy raptor claws</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8tz3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1f8tr3l</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pearly swirly nails done by me ! </t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8tr3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1f8szi4</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My biggest and only flex in life is that these are my own nails </t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8szi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1f8sgyl</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Autumn colours are creeping back in 🍂💚</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8sgyl</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1f8qwsa</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>🍋</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iostu4w83smd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1f8pvdc</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t xml:space="preserve">some of my favs nails of the year so far </t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8pvdc</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1f8p7c3</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Update: Got them shortened. </t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gkoaeo8ikrmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1f8p1h9</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pink pink nails </t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8p1h9</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1f8oztb</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>A lil messy but I’m still proud:)</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gp4nqz8uhrmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1f8owx2</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherry blossom nails 💅 </t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8owx2</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1f8o7lk</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>loving them ♥️</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8o7lk</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1f9h51n</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Is this residual gel polish or nail damage?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f9h51n/is_this_residual_gel_polish_or_nail_damage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1f9gorj</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does this pink look too dated? </t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/41ikjmlm1ymd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1f9fddj</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Remedies for brittle, curving nails?</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f9fddj/remedies_for_brittle_curving_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1f9dvys</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Maid of Honor nails 🤍</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rm2u785j4xmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1f9dirk</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Dupe for Hermès orange?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzz914nr0xmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1f9dipj</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Best nail shape for plus size girls?</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9dipj</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1f9cfdy</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Nail Bed Shrinkage</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f9cfdy/nail_bed_shrinkage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1f9ccbr</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This brings back a very specific memory </t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9ccbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1f9bymg</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ethereal’s Calcifer </t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9bymg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1f9bsno</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>End of Summer, Fall Vibes!</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9bsno</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1f9brvl</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! Why are my two nails peeling like this? </t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f9brvl/help_why_are_my_two_nails_peeling_like_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1f9b1vx</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I chose to wear this stunning polish in honor of my birth stone during my birthday week! </t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9b1vx</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1f9avfa</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Light &amp; dark nails</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9avfa</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1f9asxv</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beachside mani, nails as blue as the lake </t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/drfw65csbwmd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1f9anun</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>1422 Designs — Quiet Morning</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9anun</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1f9ams8</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Whatever brand, what's your favorite shade? I love mixing and matching but so many shades within and across brands are sooo similar </t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f9ams8/whatever_brand_whats_your_favorite_shade_i_love/</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1f9a41j</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>What in the world is going on with my nail polish?</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f9a41j/what_in_the_world_is_going_on_with_my_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1f9a0e2</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>It's not you, it's me</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9a0e2</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1f9a093</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails need healing but can’t stand bare nails! </t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f9a093/nails_need_healing_but_cant_stand_bare_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1f989qf</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>I will always be a sucker for holo</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f989qf</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1f984y4</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Nightcrawler.....wooooow...</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f984y4</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1f983s0</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Bladder Brew dupe?</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0cqdts4rovmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1f97xhp</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Trying to force it to be fall with nail polish...</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bzv41ch9nvmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1f97tph</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Shaping nails tips</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f97tph</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1f97gr3</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>blue shimmer?????</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f97gr3</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1f975pe</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Sold on Sally Hansen Gel!</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f975pe</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1f96z5n</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>🌌 Ethereal Lacquer’s See You Space Cowboy 🚬 + 🪐 Sassy Sauce’s Pain in the Asteroid ☄️</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4m05fnnkfvmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1f96hcn</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>New shifty!</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8vgyd4kobvmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1f96art</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Simple celestial ✨</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f96art</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1f9660j</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>I got inspired by a wall mural in Sacramento and my nail tech got to work! (Please forgive my cuticles and outgrowth)</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9660j</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1f95xxs</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Light/Stoney Gray Recommendations</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f95xxs/lightstoney_gray_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1f95rqk</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Fall/late summer gingham diy press-on mani</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f95rqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1f95i8f</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>China Glaze Let 'Em Roar! looks like red onion skin.</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/694cnkzf2vmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1f953ro</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>I See Dolphins</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ouhmn30d1vmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1f950ym</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>OPI My Private Jet dupe?</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f950ym/opi_my_private_jet_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1f94cr5</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What a Pretty Fire 🔥 </t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nqatgdahvumd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1f8i801</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm Becoming a Bit of a Mixologist </t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q70j5aksdpmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1f90pt8</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>My very first at home DIY manicure after years of acrylic abuse</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f90pt8</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1f90c8c</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Dupe for CG City Siren?</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f90c8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1f8zuf5</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>base coats without pvb or acrylates copolymer</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f8zuf5/base_coats_without_pvb_or_acrylates_copolymer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1f8zs2q</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>What's the New Cool Base Coat</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f8zs2q/whats_the_new_cool_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1f8znyf</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Favorite polishes you can buy in stores? </t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f8znyf/favorite_polishes_you_can_buy_in_stores/</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1f8yvcg</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>🩷💖Pink Panther💖🩷</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8yvcg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1f8ytue</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Pretty pink</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8ytue</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1f8ypl7</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>I love green 💚💚💚</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8ypl7</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1f8yl0e</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Nails for Beetlejuice Beetlejuice tomorrow!</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8yl0e</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1f8yjyv</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>INLP magic flakies over white?</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lf5pc737qtmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1f8yipb</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Granite Nails</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8yipb</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1f8y852</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>MSM Transporting me back to 2010ish</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f8y852/msm_transporting_me_back_to_2010ish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1f8y47j</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>It's Giving Candy Apple</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8y47j</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1f8xt5n</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Thought this was a cute late summer polish</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8xt5n</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1f8x958</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Looking for a nail polish dupe of Mylees "For Your Eyes Only" gel polish</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8x958</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1f8ww5u</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>She wore a raspberry parade! (beret)</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8ww5u</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1f8wpxt</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Help me figure out which one this polish is.</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kxhtgfo6dtmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1f8w9zq</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Yep, that’s purple!</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8w9zq</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1f8usw5</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP Bluebell: a shiny happy polish if I ever saw one </t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4dphnn35zsmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1f8tpmd</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>It’s giving swamp party</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mbfhj6pzqsmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1f8ths3</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Glossy Red</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/D7XczUn</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1f8tfdl</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Experimenting with Flower Child as a topper 🌸🌺🌼</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8tfdl</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1f8ru66</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Feeling like Dracula's mistress today 🧛</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iua4ndyqbsmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1f8pmlb</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Dupe for Cirque Colors Cultured?</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8pmlb</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1f9gink</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>korilakkuma set ♡</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9gink</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1f9ghi9</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m having a lot of fun experimenting with my nails </t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dbhhf20yyxmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1f9fqhp</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>The Elegant and clear nails 💭</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdq7eqelpxmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1f9exb6</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>More spoopy nails♥</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n3zzsleyfxmd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1f9e3jf</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Do you see any progress?</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9e3jf</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1f9csz2</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Made Charlie Brown Press-ons for my brother's fiancées's trip to Knott's Berry Farm. She only wears long nails on one hand, so just 5 nails.</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8bvsvfstwmd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1f9ciqt</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t xml:space="preserve">An internship I did for a gel and decoration course </t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4i6nvovzqwmd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1f9astb</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>MACHINA 👽⛓️</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9astb</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1f9ae0e</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Making sure my girls have the perfect nails to match their feminine aura💅</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ekglp7j48wmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1f99hzw</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>pink and green nails i did!</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4cifxvzj0wmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1f99frs</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Acrylic paint on nails?</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1f99frs/acrylic_paint_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1f98pgt</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>First attempt at intricate nail art</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f98pgt</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1f974ec</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Playing with cat eye gels</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hzcsyk5pgvmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1f96nqh</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>I accept all constructive opinions, I've been practicing for 2 and a half weeks 💘</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f96nqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1f94zf8</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Airbrush recommendations </t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1f94zf8/airbrush_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1f93jc5</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beetlejuice! </t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i46p7rfkpumd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1f91ze6</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>press on nails i paint on gets soft after i painting , coating etc.</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1f91ze6/press_on_nails_i_paint_on_gets_soft_after_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1f8zsa3</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best nail tips for making press one? </t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1f8zsa3/best_nail_tips_for_making_press_one/</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1f8wsli</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Retro neon chic 💛💜</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzypvp3qdtmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1f8wfmu</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>felt too down lately to do a nice set - i think i'm coming back slowly 🤗</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8wfmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1f8to7o</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Swan lake nails I did 💕💅🏼</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8to7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1f8qvdh</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>No theme</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8qvdh</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1f8q5cj</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Looking for Katakana 3D bedazzled nail charms</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s6bebatdvrmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1f8oy04</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherry blossom nails 💅 </t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f8oy04</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Sep  6 08:09:58 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_09_08.xlsx
+++ b/data/2024_09_08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C835"/>
+  <dimension ref="A1:C1018"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14628,6 +14628,3117 @@
         </is>
       </c>
     </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1fa9scl</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink and green </t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mbz5eah8b5nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1fa8sy6</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Tried brown..not sure about them</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa8sy6</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1fa8mny</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>First time doing gel nail extensions!</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa8mny</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1fa8mfg</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>New design, what do you think of the color and design?</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwuizs17w4nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1fa8ht1</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Maintenance and design change, I’m sooo proud &lt;3</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nq7y63zju4nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1fa7e0o</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>PLEASE HELP!!</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa7e0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1fa7b60</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help finding a similar color cat eye? </t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nzq4xzcng4nd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1fa851b</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t xml:space="preserve">photo of my new nails before going to school </t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6j68qf9q4nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1fa7tfd</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Random press on from Claire’s I bought today- cute or cringe??? I kinda like the design idk</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2axzisim4nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1fa6p7v</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Best for damaged nails: Gel-x vs. dual form?</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fa6p7v/best_for_damaged_nails_gelx_vs_dual_form/</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1fa6j9i</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>golden velvet nails for a wedding look ✨</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa6j9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1fa64ey</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Pr*gly Skittle 💩</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa64ey</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1fa5z8r</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>My birthday nails 💖</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa5z8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1fa5qe2</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Press one</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fa5qe2/press_one/</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1fa573y</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Lisa Frank leopard and French tips. What do y’all think?</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa573y</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1fa56e1</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Jelly nails</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/apn18xb8v3nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1fa4paw</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gt03lw4tq3nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1fa4hfk</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>My nail tech absolutely killed it this morning 🩷</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa4hfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1fa47us</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glue on nails </t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fa47us/glue_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1fa3yc0</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>What nail shape do you think would best suit my hand?</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fa3yc0/what_nail_shape_do_you_think_would_best_suit_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1fa3p9k</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails every week is exhausting </t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rau9harh3nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1fa3ock</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Cherries!</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9lklvxih3nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1fa3me8</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Does this nail shape work for me?</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa3me8</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1fa30vx</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Did the lady who did my nails do me dirty?</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa30vx</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1fa27td</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>My nails are all mismatched, which shape is best?</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa27td</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1fa2nwy</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Newest set, Vans inspired 🖤❤️💛</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yyr9eihb83nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1fa2l1x</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Starry night nails</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa2l1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1fa2jqt</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>green frenchies with some squiggles!</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa2jqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1fa2a7w</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>hello, I went and got them fixed. I just asked if they could make them smaller on the top and they did shape them a little more! thank you everyone for your comments.</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa2a7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1fa27ev</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Can’t pick one!</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa27ev</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1fa1pgd</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Clasé azul</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa1pgd</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1fa1ki6</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>What I wanted Vs What I Got 🤭</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uk18gf4py2nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1fa1ml4</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>How to remove not grown-out acrylics?</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fa1ml4/how_to_remove_not_grownout_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1fa1em6</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which nail shape suits me better based on my hands? Almond or coffin </t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa1em6</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1fa18ya</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! My nails keep breaking </t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fa18ya/help_my_nails_keep_breaking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1fa108r</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Wedding tomorrow!…</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jiqptbhyt2nd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1fa0syz</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>new nails🌸🎀</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wp36ljv9s2nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1f9znma</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1st time as a male getting my nails done at a salon! </t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9znma</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1fa0n47</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Final Summer Mani</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wbixh75yq2nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1fa0i4l</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Liquid holo</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fa0i4l/liquid_holo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1f9zwfq</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail designs I did that I thought looked cute, sweater and cherries 🍒 </t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9zwfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1f9zoqw</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in what ways can i improve how i do my press-on nails? </t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9zoqw</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1f9zees</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Potentially my favorite set of the year </t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9zees</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1f9yiuc</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>My Melody Polygel Extensions!</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9yiuc</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1f9yetm</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>💚🧡 ILNP Legacy ✨🍂 My favorite transition shade from summer to autumn. Olive green to gold to orange with a little holo sparkle ✨</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9yetm</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1f9y8p8</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i never get my nails done but for my wedding id like them and this is a trail run. however i knocked my ring finger cause the nail to bend back and pop off, should i just take the set off or glue it back on for a bit and keep them a bit longer i only got them a week ago </t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9y8p8</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1f9y8hq</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Red nails for the first time</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9y8hq</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1f9y588</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>💋❤️🥀</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9y588</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1f9y1d0</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not perfect but great $7 nails that last a week </t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9y1d0</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1f9x7cu</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Redoing my nails~~</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3g4bcdzg02nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1f9x0cz</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time filling nails at home </t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9x0cz</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1f9chus</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Divot in my nail</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f9chus/divot_in_my_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1f9wxdi</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>A lot of glitter around here today. Do you like it or should I choose another design? What do you recommend for my hands?</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9wxdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1f9wng8</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Terrifier Portrait </t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4whkphwdw1nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1f9wc92</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on nail questions </t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f9wc92/press_on_nail_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1f9vz27</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails by @atelier_nail_studios - how to identify and ask my own tech for this style?  </t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9vz27</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1f9w54f</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Giving spooky/fall vibes!???</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9w54f</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1f9vtpo</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Press on nails too big?</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9vtpo</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1f9v1dv</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Builder gel… does it cover stains on nails?</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f9v1dv/builder_gel_does_it_cover_stains_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1f9t0bk</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Alternatives to Gel?</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9t0bk</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1f9vcy4</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Mushrooms for early fall 🍄</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4c6vtg5n1nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1f9v5hx</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Advice on what to get at salon for my wedding</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f9v5hx/advice_on_what_to_get_at_salon_for_my_wedding/</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1f9v2wh</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>First time painting press ons</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9v2wh</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1f9v18s</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I usually do almond, but ive been loving long squares lately. Heres my latest manicure i did myself💗 </t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9v18s</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1f9uzm7</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>went classic &amp; simple for my engagement that’s happening sometime this weekend!! 🤭🥰</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrj39w1fk1nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1f9umd6</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got these done for 10$ </t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9umd6</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1f9ucla</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love green </t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0267620rf1nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1f9tf4x</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>My cousin did my nails. So proud of her 💖</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03gnochv81nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1f9t6jb</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t xml:space="preserve">September </t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frmewc5471nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1f9t3ht</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>What am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iueveshi61nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1f9t36j</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Last Summer Set / First Gel-X Set!</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9t36j</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1f9t2ps</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>new mani pedi</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9t2ps</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1f9snog</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Love this new set so much!</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/is01v7nc31nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1f9salq</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Black bomb 😌</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9salq</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1f9s4pi</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first time in a long time getting nails. My nails feel/look heavy, am i overthinking? </t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9s4pi</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1f9rsgg</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Aurora set</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9rsgg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1f9qzzt</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inspo from @polishedbyalyssa. My nail tech is amazing. I love black and white designs. </t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9qzzt</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1f9r023</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Crazy 3D mouth set I did !</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vsvp16xdr0nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1f9qscf</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>possible to fix?</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9qscf</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1f9qoeo</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Angry</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9qoeo</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1f9fmt4</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>I got these false nails want more but don’t know what kind they are</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tas9z2ucoxmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1f9ised</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t xml:space="preserve">replacement for gel to have sturdy nails </t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f9ised/replacement_for_gel_to_have_sturdy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1f9gocf</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Is this residual gel polish or nail damage?</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7sn0khg1ymd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1f9lz9i</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When my nail tech listened patiently to my half-baked idea about “19th century headstone iconography” 🪦 </t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zac70ydtozmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1f9ob5u</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Love a good “hooker red” nail! 😂🤪🥰♥️</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4gs3n23n70nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1f9opup</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Press on nails - what kind of fake nail to use?</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f9opup/press_on_nails_what_kind_of_fake_nail_to_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1f9prgf</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>I want to keep these nails forever</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxg1grhdi0nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1f9qbid</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cateye powder - regular nail polish - help </t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f9qbid/cateye_powder_regular_nail_polish_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1f9q5jx</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>What are the best regular nail polish collections? Europe</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f9q5jx/what_are_the_best_regular_nail_polish_collections/</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1f9oz7r</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Made these for my mom who is in her 50s😂</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zbrkgxlkc0nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1f9ow48</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loooove theeem </t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5tr1lxvb0nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1f9oo62</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My new fall manicure 💔🧛🏻‍♀️ what do you think about this design? </t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9oo62</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1f9odyw</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>First time trying gel x 🍓</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xtnmeb780nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1f9o3y0</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>UV cure jelly press-ons?</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dcearn7560nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1f9ncmy</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>I think I found the perfect nude for my skin tone ~</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/prs2gz2hzzmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1f9mwq0</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Sheer black w polka dots🖤</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jml9bau6wzmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1f9lqa6</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Looking for a post!</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9lqa6</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1f9kt46</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>made those for my friend 🙂</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wphe73kezmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1f9krsh</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>quick growth/fill time?</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9krsh</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1f9kou4</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t xml:space="preserve">doing nails for 5 months now ✨ </t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lu3re8xfdzmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1fa8q3c</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>How durable/ Long Lasting are Strengtheners?</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fa8q3c/how_durable_long_lasting_are_strengtheners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1fa7g3g</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Magnetic Nail Polish</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fa7g3g/magnetic_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1fa6x76</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>My Humble Hoard</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa6x76</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1fa62mx</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Prugly Skittle 💩</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa62mx</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1fa5vqd</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Phwoar  🦚</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/dltow0D</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1fa37gd</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Dupes for ORLY Almond Milk?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q3lhq8l6d3nd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1fa31jl</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t xml:space="preserve">good cheap jelly? </t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fa31jl/good_cheap_jelly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1fa2kug</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Ethereal Manicure 🤩</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa2kug</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1fa2ayz</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI funny bunny combinations </t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fa2ayz/opi_funny_bunny_combinations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1fa22pk</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirque lucky bag fall </t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa22pk</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1fa1pg2</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>First Indie Polish</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nbhw6lwvz2nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1fa1l0z</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>PPU- Sassy Sauce Not Your Mama's Fairytale</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhrn2dpty2nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1fa1jfh</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat - Forces Of Evil </t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa1jfh</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1fa11lx</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Thanks, Ünt. I definitely wanted my polish to pop off at random.</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtt6jfcau2nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1fa0tce</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Clionadh Psilocybin velvetized</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/azrk1plbs2nd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1fa0tep</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Final Summer Mani</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ay77868es2nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1fa0ly2</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Based on a comment I made on another post- describe the personality of your current manicure. Who are they? Where are they going? What are their pet peeves? What mistakes do they keep making? Be creative and specific! If you can, share a pic or the name of the polish!</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kpv8rnvoq2nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1fa093u</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Sea Witch</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/goyotjbsn2nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1f9z9xj</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Dam Polish - Regret Nothing</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9z9xj</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1f9z5fh</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dirty top coat? </t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edycfar7f2nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1f9z3om</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Waited all year for chocolate nails 🍫</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9z3om</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1f9ytnf</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>I did a french manicure for the first time on my left hand.... The right hand is tragic tho lol... Ignore the stray polish it will come off in the shower lol</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9ytnf</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1f9yqls</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Neutral fall favorite (OPI)</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9yqls</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1f9ydtz</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>💚🧡 ILNP Legacy ✨🍂 My favorite transition shade from summer to autumn. Olive green to gold to orange with a little holo sparkle ✨</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9ydtz</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1f9y43c</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t xml:space="preserve">TJMaxx FTW! </t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7g0wkx5a72nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1f9xwk2</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Looking for press-on recs</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f9xwk2/looking_for_presson_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1f9xsap</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t xml:space="preserve">If international shipping was easy... </t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9xsap</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1f9x66t</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Show me your Fall nails!</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f9x66t/show_me_your_fall_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1f9wrsg</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>First time using Death Valley Nails (DVN)</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/akp1rqaax1nd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1f9w11f</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Disappointing Glass Jellyfish</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9w11f</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1f9vz7s</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Covering tip-wear</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9vz7s</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1f9vvey</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>What iS The Difference Between The Two?</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f9vvey/what_is_the_difference_between_the_two/</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1f9uomz</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>🖍Crayons🖍</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9uomz</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1f9uhhl</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Favorite top coat?</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f9uhhl/favorite_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1f9tfzu</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>first mooncat polish 🤠</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9tfzu</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1f9t2fs</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>On the hunt for an emerald green creme...does it exist?</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/st67py8a61nd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1f9sy8v</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>A fun grey</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8upme8ng51nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1f9ssuw</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>I didn’t love this polish until I realized how amazing it looks under UV/black light</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23ua9xoc41nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1f9scd2</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>i think i finally found my nails but better polish</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9scd2</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1f9s3hs</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In love with this polish </t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9s3hs</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1f9s3ad</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Office lighting is the best lighting</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9s3ad</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1f9ry05</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Kur Nail Veil</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9ry05</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1f9r4mu</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Went to grab a drink after applying my base coat…</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j5jjvsebs0nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1f9qwen</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Mercury's tears</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9qwen</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1f9qt4i</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>DVN fall drop</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f9qt4i/dvn_fall_drop/</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1f9qgx5</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Amazing combo ✨</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9qgx5</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1f9qeor</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Not my normal vibe but I'm loving these</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9qeor</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1f9o8gb</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Mixed feelings about my latest manicure</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ujwwf45170nd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1f9o2i3</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help finding this color </t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5a6h4ru50nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1f9o0le</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Velvetttt</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z0gn3v7g50nd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1f9mpwl</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>She seems to approve of this polish, DND gel Forgetten Pink</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2w2in8a2uzmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1f998xi</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Random Mooncat Preauth??? </t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f998xi/random_mooncat_preauth/</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1f9m4p4</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Swatcher Question</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f9m4p4/swatcher_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1f9ls79</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Flakie topper galore</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j1yekwf7nzmd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1f9lr1d</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Anyone know any dupes for Essie Sweater Weather?</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ifrkbv7ymzmd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1f9ja5t</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Kleancolor Gel Effect - new formula - Have you tried it?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ligx2isjyymd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1f9had5</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Base coat recs?😩 I seriously think there’s something wrong with my nails</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f9had5/base_coat_recs_i_seriously_think_theres_something/</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1fa8ng3</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Was $200 spent on My first fall manicure, worth it?</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48tuun9zv4nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1fa8lsz</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>I feel like I'm different from the girls around me.</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gz3cd8mpv4nd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1fa77m6</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>my new decor nails: classic french tip meets halloween twist</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cltr12p6f4nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1fa6dts</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Because actually my job... is just Beach </t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa6dts</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1fa3m08</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm learning how you rate my nails girls </t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gxmrvz5xg3nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1fa3hsf</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Mommy&amp;Daughter nails 🤍</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgaup97uf3nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1fa2ltd</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Starry night nails</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa2ltd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1fa1sby</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Bridal set; hand sculpted 3d builder gel</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fa1sby</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1fa0b53</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Sea Witch</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ntc7mz8o2nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1f9zhaa</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Nude 💅</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9zhaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1f9z1a3</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>French Tip with Zebra stripes and a vertical ombre</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9z1a3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1f9yt8u</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>How do I do this?</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9yt8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1f9ymgw</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>My Melody Polygel Extensions! Criticism Is Welcome</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9ymgw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1f9vud4</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>how can i make the finished press on nails harder / more durable?</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1f9vud4/how_can_i_make_the_finished_press_on_nails_harder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1f9vs4c</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Cute butterfly’s my wife made last night !</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9vs4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1f9vr6y</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Witchy &amp; Glittery! 🖤🧡</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9vr6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1f9uiun</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Did some clown inspired nails🤡</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzuup64zg1nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1f9u88q</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>work in progress for a halloween set 👁</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9u88q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1f9tsfs</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Black, white &amp; silver 🖤</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rlnhqh3mb1nd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1f9tg7z</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail tech did these for me today! (She does not want to be credited on Reddit as she's only 17) </t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9tg7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1f9s2r7</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>What should I do for the plain green nails?</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tqngito5z0nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1f9rr9c</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Aurora set</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9rr9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1f9nqly</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>silly lil guy I painted 😋</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c694hxxy20nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1f9mu45</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Autumn/halloween inspo </t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9mu45</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1f9lj9g</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Zebra French Tip Nails</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9lj9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1f9hh9i</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink &amp; snakes </t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9hh9i</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Sep  7 08:08:32 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_09_08.xlsx
+++ b/data/2024_09_08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1018"/>
+  <dimension ref="A1:C1212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17739,6 +17739,3304 @@
         </is>
       </c>
     </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1fb1g7h</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Let's talk DIY gel manicures.</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fb1g7h/lets_talk_diy_gel_manicures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1fb06l3</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Made this Totoro press-on set for one of my girlfriends!</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ctub9zn8ubnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1fazihk</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Gel Polish that’s Like Mooncat?</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fazihk/gel_polish_thats_like_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1faz8sf</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>What to do with dry nails?</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4o3x5fdjbnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1fayxfk</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hyper Realistic </t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fayxfk/hyper_realistic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1fay0vg</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>best nail tips?</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fay0vg/best_nail_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1fayw96</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Love this design I ordered for my holiday🌊</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hgbiff4hfbnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1fayh8j</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherry red nails, literally </t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fayh8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1faygy9</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>My nail tech never disappoints me!</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0sbeeywabnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1faxvb8</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Let my nail tech do whatever 🥰</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d64gcqau4bnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1faxlqo</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Nails at home or switch manicures??</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1faxlqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1fax39w</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Trying press on nails for the first time</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fax39w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1fax1x4</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Nude chrome nails 🤎✨</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fax1x4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1fawz76</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>I am a nail hobbyist and I post my nail art anonymously online</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fawz76</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1fawy5o</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>New press on set!</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fawy5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1faw9rr</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Should I do something about this relatively small split?</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ukf8pik4pand1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1favosm</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>best gel polish?</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1favosm/best_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1favlpz</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Hella Handmade Creations- Alibi</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1favlpz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1fauvpt</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>✨☕️</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tutvx0zzband1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1faucv1</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>love the colors in this whole pic</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hnqrm9nt6and1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1fau91z</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Painting soft gel tips before application?</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fau91z/painting_soft_gel_tips_before_application/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1fau84u</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>My friends cute Hello Kitty Nails 🩷🩷🩷🩷</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fau84u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1fau161</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>💜✨❤️</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vv2ah6j54and1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1fatmsm</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Please help me :( First time nails and so much discomfort </t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fatmsm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1fatun5</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>It's almost time... 💀👻</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ln9w1dl2and1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1fatsda</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>What iS The Difference Between The Two...?</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fatsda/what_is_the_difference_between_the_two/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1fatosm</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>My first set of dip powder I done on myself, let's just say I need more practice.</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5kgl2d171and1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1fatjwm</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>some fairy nails i made for a friend back in june! :)</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sjv79pm10and1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1fatjsg</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Fall French</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axfw1rd10and1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1fathgl</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Fall nails ☺️</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jmb0p04hz9nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1fatexe</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>First Attempt at Torties!</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wjtdvt1vy9nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1fat5si</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Spooky season is upon us 🦇</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fat5si</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1famutm</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Zebra stripes over French Tips and a vertical ombre.</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izwcjrsqj8nd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1fastpv</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fastpv/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1fas3up</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Monet Nails</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1bgbit3tn9nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1fas0zu</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Colorful Blobbies - Nails</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fas0zu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1farvch</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Loving the matte with shiny tips combo def gonna do it again with a different color</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cq24btbzl9nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1farn4y</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Second press on attempt </t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1farn4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1farhcq</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>What do you think? Take it easy, I'm learning.</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1farhcq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1farh6p</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>What do you think? Take it easy, I'm learning.</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1farh6p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1fard7y</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>I love my hello kitty nails !</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmz0s8tzh9nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1faqvi2</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Should I just cut the rest off my nails and grow them all out again?</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5rm5i2r3e9nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1faqab1</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>is it okay to get your nails done with bitten nails?</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1faqab1/is_it_okay_to_get_your_nails_done_with_bitten/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1fapxfu</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>some coraline inspired nails i made for a friend a couple of months ago!</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/usv2lkpo69nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1faq0aw</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Thoughts? :)</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jyqocrdb79nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1fapz46</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>diy press on nails</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fapz46</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1fapg26</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>What celebrity do you think has the best nails?</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fapg26</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1fapay5</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>I want to get pretty nails, what do you suggest?💗🤔😗</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/biqp9rvg19nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1fap7vh</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Teabag method working well</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fap7vh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1fap5qw</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Flower Gem Nails</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fap5qw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1fap23f</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>2nd set of gel x</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fap23f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1fap01v</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Lava Lamp Nails</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kle54hflz8nd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1faozbl</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>3D Funky Grunge Nails</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u5r12l5ez8nd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1faoy6v</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>🐰🎀</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7c22qorbz8nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1faoy1y</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Icy Nude Aurora Nails</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1faoy1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1faoxxd</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Gel on natural nails</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1faoxxd/gel_on_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1faoxe5</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>3D Cute Halloween Nails (Color-Changing)</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pzvnmbpzy8nd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1faovsq</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Pastel Pink Floral Nails</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y2twxfnmy8nd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1faotw3</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>NEVA PLAY by Megan Thee Stallion Inspired Nails 2.0</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3jo5o3cy8nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1faotsz</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails to see Beetlejuice Beetlejuice tonight 🪲 </t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1faotsz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1faot6e</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I use builder gel to attach press-ons? </t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1faot6e/can_i_use_builder_gel_to_attach_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1faosss</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Birthday nails✨</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0268ngu6y8nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1faosnh</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Nails Inspired: NEVA PLAY Music Video by Megan Thee Stallion</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3rsvy27xx8nd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1faoqfz</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Coffee Aurora Nails</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wuqamkoix8nd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1fanrt3</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what is a good nail strengthener brand that’s hema and acrylate free ? </t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fanrt3/what_is_a_good_nail_strengthener_brand_thats_hema/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1faod9s</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>How to get my gel nails off of my natural nail?</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1faod9s/how_to_get_my_gel_nails_off_of_my_natural_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1faoc7x</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Turquoise effect</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ayqez8dvu8nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1fanz7s</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I feel like such a fraud in the nail salon with my grocery store nails </t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u6g7htg7s8nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1fanaxl</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Deborah Lippman “you can leave your hat on”</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fanaxl/deborah_lippman_you_can_leave_your_hat_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1fan9xc</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My embarassing attempt at press-on nails. 💅🏼 </t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1xmaceum8nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1famll7</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>I got a barbie french manicure</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1famll7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1famgxh</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>First attempt at DIY Gel X Nails</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1famgxh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1famdh6</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>ILNP - Be Mine</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1famdh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1fam9jl</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Getting ready for the fall w these cuties </t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7tnc5j6f8nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1faltvt</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>“Glamnetic” press ons I got today. New to the world of press ons- any tips and tricks to keep them on, or in general? Thanks! 💖😊</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1faltvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1faljay</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beetlejuice 🪲 </t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1faljay</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1falepi</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>My 2nd nails</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnkf6yvr88nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1falbo7</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Cinnamoroll French tip set 🩵🥰</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1j9pqx488nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1faky40</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>My nail and flower</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gho5xwy958nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1faksuq</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>New set 🤎</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wym5873748nd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1fakac8</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>At home gel nails with chrome</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fakac8/at_home_gel_nails_with_chrome/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1fak2m7</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help me keep my nails from bubbling </t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fak2m7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1fajqik</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Are fast growing nails thinner?</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fajqik/are_fast_growing_nails_thinner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1fak1wa</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>I went to get my acrylic nails removed and I feel uneasy about the way they did it?</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fak1wa/i_went_to_get_my_acrylic_nails_removed_and_i_feel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1faircz</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Welp. That was dumb.</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wsdeaeqzo7nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1faijey</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set ✨ </t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1faijey</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1fajfw2</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Friday date night nails</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fajfw2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1faiyf3</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lace nails I did on myself </t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oag9pb5dq7nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1faitkk</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Simple but cute</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1faitkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1faif38</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">❤️ </t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1faif38</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1fai03o</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set 💚 </t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5gy1zfbj7nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1fahup8</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set. Do we like the shape? </t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fahup8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1fag4vy</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>One year since my first attempt at a gel manicure 🥳</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fag4vy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1faca7q</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help!! How do I get paint from out under gel x nails? </t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1faca7q/help_how_do_i_get_paint_from_out_under_gel_x_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1fab3z8</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ISO inspiration/ideas </t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fab3z8/iso_inspirationideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1fage30</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>This is why I can't have nice things 😭</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fage30</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1fag7v8</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opinion wanted </t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fag7v8/opinion_wanted/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1fafqrv</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>8 years since my last set of stilettos</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/moc0yc8a27nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1fafcsc</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Velvet rose by mooncat cateye</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fafcsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1faex6s</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Always fun doing my tattoo artists nails! </t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwivyg5mv6nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1fb0tab</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Finally figured out stampingq</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fb0tab</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1fb07xk</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help identifying these opi shades </t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7o6twqnubnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1fayna5</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Eyeshadow for coloring nail gel</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fayna5/eyeshadow_for_coloring_nail_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1fajuj0</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cant find the real shade name </t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fajuj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1fajmh7</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer’s La Ciudad Más Hermosa del Mundo</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eupp7pjbv7nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1faja98</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Painted my husband's nails for Beetlejuice Beetlejuice!</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lka2ecqrs7nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1faygy6</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Searching for “the perfect neutral”</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1faygy6/searching_for_the_perfect_neutral/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1faxs4m</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>A simple palette cleanser 🤎 I'm glad that I chopped, and I'm loving almond!</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1faxs4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1fawgh2</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Do all indie brands use the same suspension base?</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fawgh2/do_all_indie_brands_use_the_same_suspension_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1favtct</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Emily de Molly: Get in Line</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zhhogmorkand1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1favk5j</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Hella Handmade Creations- Alibi</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1favk5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1favag9</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>I Haven't Done My Nails In a Month</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1favag9/i_havent_done_my_nails_in_a_month/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1fauykm</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>✨☕️</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0x4vx6pqcand1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1faupcb</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>It means no worries</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1faupcb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1faumsu</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One gel-x nail always lifts/comes off first. </t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1faumsu/one_gelx_nail_always_liftscomes_off_first/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1fatwvn</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>[bare nails] Nail polish accidentally peeled off &amp; damaged my nail, how to I save it?</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/noi4p7243and1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1fatq9o</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Carrie - Cupcake Polish PPU </t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fatq9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1fatnin</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Goosebumps inspired polish? Yes please!</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fatnin</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1fatn3e</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>I've never stared at my nails so much with just a creme manicure</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fatn3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1fati0z</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Looking to re-create this LP album art on my nails- looking for tips!</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fati0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1fasyu3</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>You’ve Got Nail</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fasyu3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1fasy35</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! Is this color yellow or orange? </t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cjlaulzvu9nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1fasooc</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Dollar Tree chrome powders!</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fasooc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1fase3k</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Moody oxblood for fall 🥀🩸🖤</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fase3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1farw2k</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matte nails with shiny tips </t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rdo6lm65m9nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1faril8</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Poison Ivy</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1faril8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1far8mo</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Matching my nails to my jewellery creations 💚</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pr71jia0h9nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1far26r</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>this thermal!! she has the range!!! (Cat Tail Nails - Bloody &amp; Bruised) (PPU Rewind ‘24)</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1far26r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1faqem7</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Lacquer repair?</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1faqem7/lacquer_repair/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1faqb6u</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>It's 111° right now! 🏜️</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1faqb6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1faq0hw</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Getting nail polish to stick to my nails?</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1faq0hw/getting_nail_polish_to_stick_to_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1faprja</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Magnetic Nail Polish</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1faprja/magnetic_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1fapn4c</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Grungy Jewel Tone</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fapn4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1fapkrw</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone know of toppers with colorful matte dot glitter / speckles? Like these but with smaller dots. </t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fapkrw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1fap725</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Another temperature changing polish! Vivid blue version! (Dark blue when cold, light blue when warm!)</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fap725</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1fap1pm</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Facebook Marketplace hauls: Londontown, Essie, Orly, Morgan Taylor </t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fap1pm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1faokj3</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Autumnal skittle 🍁 </t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1faokj3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1faocrm</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ocean Ombré </t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xs3qc0jzu8nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1fao6oz</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>LynnB DOES👏NOT👏MISS👏</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fao6oz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1fanujn</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The set I got for Pride the other month. 🌈 </t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/les7os88r8nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1fancl3</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Deborah Lippman “You can leave your hat on” </t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fancl3/deborah_lippman_you_can_leave_your_hat_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1fanbm2</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall skittle! </t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fanbm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1famuzf</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Shh, I'm Fabulous</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1famuzf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1famf7g</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>ILNP - Be Mine</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1famf7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1fam8ma</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Another PSA to check your local dollar tree!</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8i8sabkze8nd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1fam61w</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Finally got my hands on the Nightlife collection from ILNP and it does NOT disappoint 😍😍</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y7e3z4yfe8nd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1falij8</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Clionadh Hot Toddy ✨</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yvn505ok98nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1falckk</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Dark green lighter than Off Tropic?</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1falckk/dark_green_lighter_than_off_tropic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1fal21l</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Safe activator? </t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fal21l/safe_activator/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1fakg1j</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Essie's "No Chips Ahead" top coat is quite litterally the worst</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fakg1j/essies_no_chips_ahead_top_coat_is_quite/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1fakem8</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Lyn B - Don't put me down for mummification</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fakem8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1fajd2c</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Any SA lacqueristas🇿🇦 ?</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xy7os0hct7nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1fajbk2</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Idc if it’s still 90 degrees out, September means fall!!</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ln14sj1t7nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1faj52x</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Phoenix -Eclipse day 5 renewal</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/47hphgvpr7nd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1faj33o</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Dupe request: DVN Sumac (discontinued)</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tohlbpa9r7nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1failby</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>It’s fall bc I said so!!</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1failby</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1faifuv</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One of my favorite turquoise shades! </t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1faifuv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1faicsn</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Late Summer Sparkle</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1faicsn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1fahd1f</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat Earth to Gaia </t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fahd1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1f9xoqe</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Celebrating not picking my cuticles anymore!</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f9xoqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1fafkix</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(Paid) Sour Grapes coming to Drunk Fairy Polish 9/13 </t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fafkix</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1faghz9</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looks way better live than on camera... </t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2qf72e787nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1fafncd</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>I wish that's all that I spent on my knitting.</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yje1k0qjx0nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1fafg6p</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Question for the magnet loving ladies ...</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fafg6p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1fafafb</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Anyone able to do a comparison between BKL’s Praise The Shaggy Dog and Ethereal’s A Heart’s A Heavy Burden?</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fafafb/anyone_able_to_do_a_comparison_between_bkls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1faf4bt</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherry Pineapple Popsicle </t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1faf4bt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1fad9ap</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>What was your first PPU order?</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/gdEA2ah</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1fad4al</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>New DVN collection complete catalogue of swatches</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fad4al</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1faccls</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>First time painting my nails in 4 years.  No acetone to clean up with and I got into a stupid argument with my wife afterward, but at least my nails look sparkly-cute.</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edbajuoo76nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1faauso</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>In search of Crackle nail polish</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1faauso/in_search_of_crackle_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1faakdl</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Kiko Nail Polish</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwdrv75ol5nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1faa19p</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Dupes for Essie Petal Pink?</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1faa19p/dupes_for_essie_petal_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1fb0pqj</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Bahama Mama Nails</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fb0pqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1fazxs0</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Freestyle Nails by me</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fazxs0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1fawz6f</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>I decorated some press ons!</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c42a86jzvand1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1fav64j</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>hand made cat eyes nails, green or blue?</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vkfa056neand1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1fauo8n</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sea decoration </t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/54oqbxt1aand1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1fau8dt</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t xml:space="preserve">thanks to everyone in r/NailArt i was able to make my first set of press on nails ever! </t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fau8dt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1fatc3v</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Comic nails </t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uy1jupr6y9nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1fat3n7</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best image editor to create full page of custom stickers or waterslide decals from high res images, without quality reduction? </t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fat3n7/best_image_editor_to_create_full_page_of_custom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1fat0vo</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Lemons by the Sea</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7udy9aijv9nd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1faszm2</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>My nails now</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1faszm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1fartmc</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Some nail designs I’ve done the past few weeks 💅🏽</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fartmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1fal3iq</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>End of summer set 💅🏿</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fal3iq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1fakh8v</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Honest opinions </t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fakh8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1fak5ls</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>How did they turn out?</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5q3c6ylbz7nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1faj1re</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time. I feel like a princess 👸</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1faj1re</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1fag3sc</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Last weeks sets ✨</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fag3sc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1fafrqz</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>A bit of marble effects</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fafrqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1faf7k0</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>I love matte colors</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bajw455zx6nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1fae3dj</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Still learning! </t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fae3dj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1fadkeg</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Getting into nails, advice?</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fadkeg/getting_into_nails_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1faaz8o</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>I love my cat, so I did a diy manicure to match it</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgqz9661r5nd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1faanbp</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Honest Opinions</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1faanbp</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Sep  8 08:08:46 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_09_08.xlsx
+++ b/data/2024_09_08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1212"/>
+  <dimension ref="A1:C1379"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21037,6 +21037,2845 @@
         </is>
       </c>
     </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1fbrhbo</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Navy and stars</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbrhbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1fbqsl2</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>First time using builder gel on nails</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gkooa7vkxind1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1fbqew9</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Reminds me of valentines but its almost Halloween </t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/15qrlo8xsind1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1fbpy7d</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best Nail Shape - Short Nail Beds? </t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ck72gzlknind1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1fbpy35</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Devil on my shoulder 😈 </t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/827gypyinind1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1fbppdg</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pale girlies </t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v82ym4kskind1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1fbokj1</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm having doubts my thumb nail is going to grow back. </t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fbokj1/im_having_doubts_my_thumb_nail_is_going_to_grow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1fbozd7</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Builder gel</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fbozd7/builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1fbn57l</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lifting or flooded cuticle? </t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6a0ipl2nthnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1fbn3uh</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Red Matte Nails I did myself</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbn3uh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1fbml42</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>My little friends glowing in the dark 👽</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbml42</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1fbm9im</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>New nail tech nailed it!</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbm9im</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1fbm2yk</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>I finally found a salon that does more than stickers for nail art!</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbm2yk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1fbm1eb</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Apex?</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbm1eb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1fblvk4</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>😻🤎</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxmxfp26hhnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1fblp1b</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Too early?</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hbuna5efhnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1fbll95</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Simple Short Black Nails</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r377rjleehnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1fbledq</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>How ro remove gel nails on toes?</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fbledq/how_ro_remove_gel_nails_on_toes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1fbky3g</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Nails sun kissed ♡</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9uqr1kc8hnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1fbkxh2</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying out cat eye! </t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbkxh2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1fbkldg</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I do my own gel and dip nails. This is my first time playing around with magnetic cat eye gel and sheer jelly colors. Silver cat eye and teal jelly over it. </t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h9r9bc275hnd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1fbklui</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing my own gel nails </t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9hycd08e5hnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1fbkc3d</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Y'all want a sprite cranberry? (cherry)</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihorgmpy2hnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1fbk73n</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Paint over gel nails</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fbk73n/paint_over_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1fbk4so</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>pop rocker ✨📀</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7oqbsi71hnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1fbk4fu</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>On this day a year ago. Came pretty far….</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbk4fu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1fbjzwj</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Extra nail extensions and press on nails</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyirw4s10hnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1fbjxmv</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pedicure progress </t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbjxmv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1fbjoxr</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Did my mothers nails</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/quwe8zqfxgnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1fbj5x2</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Lil ombre moment</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fuqarpdxsgnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1fbj128</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love my new nails </t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f8vm8gjqrgnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1fbio97</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Is this a good manicure for $47?</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbio97</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1fbhp78</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I usually love Glamnetics but their ruby red ones aren’t sticking for the life of me. Anyone else? </t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hzifl3bmggnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1fbg0za</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do I remove these 3D hard gel designs and BIAB base? </t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0psce26s2gnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1fbi6ic</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How they look ! </t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jewx1whjkgnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1fbg634</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Help with splitting nails!! 😵‍💫</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbg634</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1fbi2hf</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>New short pink nail set. What do you think, guys?</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e3f0oy11ignd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1fbdg02</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>cuticle peeling</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5bj5uzpgifnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1fbhy93</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Red passion</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s6nrp5ypignd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1fbhw4v</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red passion </t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/inzayki8ignd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1fbh1u0</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My last summer hurrah </t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbh1u0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1fbgvfg</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wine Red French Tips </t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbgvfg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1fbgu97</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>New set✨</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53ar3c4e9gnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1fbgt0c</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>I spilled three good glug-glugs of Revlon Street Wear "Raw" on my grey carpet and was able to quickly clean it pretty well using OBN sweet orange "flavor" oil-based nail polish remover pads. (stain located under products) So shoutout to OBN! I'm not even telling my husband about this!</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8y9dap8b8gnd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1fbgqx0</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dark Scarlet and Black ombre set. Happy September! </t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ypsqkbln8gnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1fbgok8</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>can i put any sort of fake nails on?</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ceuvdra48gnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1fbgm2m</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do I drink Arizona because I love this color or do I love this color because I drink Arizona (unintentional!) </t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbgm2m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1fbghj3</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>I have a small and wide nail bed. Are they okay? (Pls be nice)</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tcrnjd2j6gnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1fbghax</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Looking for a decent nail drill</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fbghax/looking_for_a_decent_nail_drill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1fbg9yv</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Would you guys cut them or keep them?</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbg9yv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1fbfvbw</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Beckoning Butterflies</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbfvbw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1fbf89g</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Recent Nails</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbf89g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1fbeo32</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>My nail tech is a keeper!</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbeo32</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1fben52</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Colorful Blobbie Nails</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fben52</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1fbemd0</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Gold Geometric Jelly Nails</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wdn8q1ogrfnd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1fbeiv1</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>fun freestyle</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xra43ovvqfnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1fbd8ou</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Best e-file for small hands nail tech?</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fbd8ou/best_efile_for_small_hands_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1fbd0ta</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Nail care</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fbd0ta/nail_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1fbcs9z</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Stunning Chrome &amp; Gold Seashell Nails! 🤩🐚✨️</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/riuqs71bdfnd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1fbcqj9</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>It’s fall y’all🍃🍂🍁</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbcqj9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1fbcg2b</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Holiday nails! 🌸🌞🫶🏼</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x66w211nafnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1fbcm9t</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural nails </t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgmd9lnzbfnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1fbb8tr</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>My nails need renovation, can you help me choose the next design?</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbuhcpc91fnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1fbcfmx</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Can I add chrome powder myself?</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fbcfmx/can_i_add_chrome_powder_myself/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1fbcb0k</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Tiny Hearts</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4yxugsi9fnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1fbc4ma</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>New Set</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbc4ma</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1fb2c00</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Anyone have pics of nail sets with uneven nails?</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fb2c00/anyone_have_pics_of_nail_sets_with_uneven_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1fbbrsb</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Nail update</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbbrsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1fb1jv8</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Growing out damaged nails</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wt7g5ijbcnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1fb1ulc</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Post mental breakdown nails ✨️</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fb1ulc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1fbayug</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>I miss my glue on’s</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tud93v2zend1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1fbat23</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>my nail tech killed this one ❤️✨</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbat23</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1fba2tp</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm in love with my new tech. Her first time doing tortoiseshell! </t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b39q4d8csend1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1fb9ihq</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>A few questions about gel nails</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fb9ihq/a_few_questions_about_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1fb9e01</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>New homemade set ✨💅</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fb9e01</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1fb97fo</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>I wish you guys could see how sparkly this polish is 😟 no</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fb97fo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1fb7sl8</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>My favorite nails</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fb7sl8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1fb8l7m</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Any fast tips to relieve pain from sore cuticles</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fb8l7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1fb95mi</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Single coat vibrant color help</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fb95mi/single_coat_vibrant_color_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1fb90oa</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>New nails, in Mexico is really cheap compared to the US</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujq10ti4kend1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1fb90ja</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Autumn/Fall Nails #1</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fb90ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1fb8znp</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Mallard 🦆</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fb8znp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1fb8s1k</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Fall but make it ✨WITCH✨</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zhxsobl9iend1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1fb8rpt</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Short Nail Season</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/is7dw2s6iend1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1fb8h6p</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Affordable UV nail glue for extensions?</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fb8h6p/affordable_uv_nail_glue_for_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1fb5ahp</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>How to ‘fix’ ski jump nails</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fb5ahp/how_to_fix_ski_jump_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1fb1mti</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Can I use drugstore gel brands with YN curing light</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fb1mti/can_i_use_drugstore_gel_brands_with_yn_curing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1fb81qm</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first time trying nail art </t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fb81qm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1fb7k32</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Perfect fall transition press ons</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7fgzohqf8end1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1fb74gr</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Pink pearl polka dots 🥰</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/grqbny7m4end1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1fb74cn</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Had a new artist….</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fb74cn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1fb73ad</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The much anticipated Virgo-botched nail update </t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fb73ad</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1fb6yqq</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>trouble with painting nails basics</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fb6yqq/trouble_with_painting_nails_basics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1fb6vwq</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ztn1k64h2end1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1fb6ufx</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>HELP, How to take gel off at home? First time doing it.</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5b1xee042end1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1fb67po</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Its my 1st time to have a softgel nails. Its really pretty!</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m6ewo7zyvdnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1fb65qk</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Winter vibes ❄️✨ Loving these frosty, glittery nails—perfect for a chic and icy look!</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mpbcaj7rvdnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1fb5z7e</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ombre with stars </t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fb5z7e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1fb5xou</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Spotted these flowers on my walk home from the nail salon</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xy43nt0ltdnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1fb4fjd</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Addicted to funky designs</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/et3ngkdpddnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1fbq4v3</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Carrying case for polish? Recs </t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fbq4v3/carrying_case_for_polish_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1fbp8ck</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Having trouble getting nails to dry if I use a topper </t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fbp8ck/having_trouble_getting_nails_to_dry_if_i_use_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1fbp66e</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Looking for a super glossy/shiny/smooth topcoat</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fbp66e/looking_for_a_super_glossyshinysmooth_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1fbozse</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Did my nails instead of the dishes. No regrets.</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rla3ouqycind1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1fblxzb</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Trying to get better at gradient but it’s hard! Do these look terrible?</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xssxbj3shhnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1fblltt</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Willow by ILNP</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fblltt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1fblhnt</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>We still doing chrome? I’m still doing chrome. 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w89r03ogdhnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1fbl4p2</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Can anyone help me find something similar in shade and opacity? I tried Essie’s jelly gloss buttercup but it was too yellow and I wasn’t a fan of the formula.</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/eiGxXQE</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1fbky3x</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>You can’t always trust the bottle (but in a good way)</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbky3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1fbkxhj</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Dashing Diva in Limone</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/joaz20dc8hnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1fbkg5b</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>How do I put on magnetic nailpolish?</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fbkg5b/how_do_i_put_on_magnetic_nailpolish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1fbkdsa</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>I love the shiftyness. Zoya Raven and Dance Legend Sulley at the tips</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/chp2lrtc3hnd1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1fbk4no</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Accidentally matched my nails to my bags today </t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbk4no</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1fbjz3r</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Amanita Moment with these Glittering Dunes</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ektfks7vzgnd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1fbjspe</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Tips peeling since I started using polish again?</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fbjspe/tips_peeling_since_i_started_using_polish_again/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1fbjm3m</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Tried the Trendy combo!!!</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbjm3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1fbj4xy</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>It’s 31 degrees where I live but I’ve decided it’s autumn anyway</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jm6eye3psgnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1fbh31a</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Dupes for Opi Germanicure from 2012?</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/clnqclpfbgnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1fbgzq8</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Iridescent silver comparison </t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fbgzq8/iridescent_silver_comparison/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1fbgvhi</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>I just feel better with confirmation... Combining topcoats</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fbgvhi/i_just_feel_better_with_confirmation_combining/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1fbgo7q</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Wrong sub to ask, but sometimes I wonder if I have a problem…</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9rphu4d18gnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1fbghqf</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Saying Goodbye to Summer Nails ... </t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/55k7cyrk6gnd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1fbge5o</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Team square, almond, or other and why?</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbge5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1fbg91b</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I Made A Promise, Mr Frodo </t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q29x318k4gnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1fbftg1</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Weekend nails 💙</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbftg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1fbfokh</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When does nail polish expire? </t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fbfokh/when_does_nail_polish_expire/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1fbfi86</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A Heart’s a Heavy Burden </t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbfi86</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1fberd2</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Trying to show the glow is just not possible…</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fberd2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1fbejng</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Soaking removal </t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f86jcq73rfnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1fbedk1</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do these work how they’re portrayed? </t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r8bbp2rspfnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1fbdrdl</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>25 lbs horseshoe magnet - initial magnetization and 24 hours later</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wv32qhlxkfnd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1fbdmc2</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🕷 vs. 🦞 </t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbdmc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1fbd1cj</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Simple Yellow Flowers</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbd1cj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1fbcs0s</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>A severe case of TTP (trust the process)</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbcs0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1fbbt81</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>this month’s nails: august 🌊</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbbt81</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1fbb4lj</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>The many faces of Disco Witch as a topper</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/va8yd5qc0fnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1fbaltn</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Vamp 🦇</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbaltn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1fba2gz</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Forget polish thinner, is there a polish thickener?</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fba2gz/forget_polish_thinner_is_there_a_polish_thickener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1fb7yaw</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>My nail broke, and it took all the nail polish with it 🥲</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fb7yaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1fb7x2e</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>🧪✨🌈 The Science of Nail Polish: curing versus drying, and what else would you like to hear about?</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fb7x2e/the_science_of_nail_polish_curing_versus_drying/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1fb777k</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Today’s experiment: I want my nails to look like sweets!</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fb777k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1fb722v</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Galaxy nails!</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kz2nw4yu3end1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1fb5cej</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>On Saturdays we wear red ❤️</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zeaoa7jqndnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1fb4809</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Solid nail glue with gel-like viscosity is that no UV cure lamp needed?</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fb4809/solid_nail_glue_with_gellike_viscosity_is_that_no/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1fb2tkf</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>This week’s mani was too cute not to share</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7nszapmvscnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1fat127</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Engagement Mani 💍 (plus my August roundup)</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fat127</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1fb2iv8</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>ISN Be Fierce &amp; Phoenix Freda 🪲🐦‍🔥✨</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3dj4ugyuocnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1fbpyhd</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Devil on my shoulder 😈 </t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jwesd87onind1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1fbpv8z</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>3D Flower designs🌸✨</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbpv8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1fbpt5m</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>finished my second set ever!!</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r97kpkuylind1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1fbp64z</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just a goodbye to summer nails </t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c7i9gzgteind1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1fboutt</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Red + Blue/green sparkle + Blue tip for fire inspo look 🔥</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hn0oqgjhbind1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1fbnwoz</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Moon Walk by CB Nails</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1piux5qa1ind1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1fbnj6z</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Coquette-ish set im working on right now, how does it look? </t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6a6njrfxhnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1fbkpxi</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Our Black Earth gel nail creation </t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/akppqcsf6hnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1fbkls8</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Dragon Nails</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o81hgamd5hnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1fbkeok</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Fresh set ❤️🖤💅🏼</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/001g8hbl3hnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1fbjsua</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Favorite set on my bf so far</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hrdwq7sdygnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1fbhg0y</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>New glow in the dark set my wife made</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbhg0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1fbgj3c</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Pierced Nails | Gothic Design 🖤💅🏻</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbgj3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1fbfeyb</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>quick set for the start of fall — gel on natural nails!</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/klzmxrq0yfnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1fbeb8e</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I want to get more connected to Nail Artists on Insta! </t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fbeb8e/i_want_to_get_more_connected_to_nail_artists_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1fbdmzh</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>woodland press ons</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fbdmzh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1fbcdt6</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherry leopard </t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wal37bw4afnd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1fba7xa</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm in love with my new tech. Her first time doing tortoiseshell! </t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hv0d0z9htend1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1fb931d</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>My first attempt at 3D nails! These are press ons with an orchid theme.</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dkac2pdlkend1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1fb83sw</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Groovy little ghosties 👻🧡🌼</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5tb2xabvcend1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>